<commit_message>
remove nan and duplicate module codes from clean_timetable
</commit_message>
<xml_diff>
--- a/data_analytics/data/Fixed_B0.02 B0.03 B0.04 Timetable.xlsx
+++ b/data_analytics/data/Fixed_B0.02 B0.03 B0.04 Timetable.xlsx
@@ -9,7 +9,6 @@
     <s:sheet name="B0.02" sheetId="1" r:id="rId1"/>
     <s:sheet name="B0.03" sheetId="2" r:id="rId2"/>
     <s:sheet name="B0.04" sheetId="3" r:id="rId3"/>
-    <s:sheet name="All" sheetId="4" r:id="rId4"/>
   </s:sheets>
   <s:definedNames/>
   <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -106,39 +105,8 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Mollie</author>
-  </authors>
-  <commentList>
-    <comment authorId="0" ref="I14" shapeId="0">
-      <text>
-        <t>Mollie:
-COMP41450 = 35
-COMP30120 = 108 </t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="B31" shapeId="0">
-      <text>
-        <t>Mollie:
-COMP30520 = 60
-COMP41110 = 19</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="G31" shapeId="0">
-      <text>
-        <t>Mollie:
-COMP30520 = 60
-COMP41110 = 19</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="65">
   <si>
     <t>B0.02</t>
   </si>
@@ -333,45 +301,6 @@
   </si>
   <si>
     <t>COMP20010</t>
-  </si>
-  <si>
-    <t>Week 1</t>
-  </si>
-  <si>
-    <t>Students registered</t>
-  </si>
-  <si>
-    <t>Week 2</t>
-  </si>
-  <si>
-    <t>Mon 2 Nov</t>
-  </si>
-  <si>
-    <t>Mon 9 Nov</t>
-  </si>
-  <si>
-    <t>Tues 3 Nov</t>
-  </si>
-  <si>
-    <t>Tues 10 Nov</t>
-  </si>
-  <si>
-    <t>Wed 4 Nov</t>
-  </si>
-  <si>
-    <t>Wed 11 Nov</t>
-  </si>
-  <si>
-    <t>Thurs 5 Nov</t>
-  </si>
-  <si>
-    <t>Thurs 12 Nov</t>
-  </si>
-  <si>
-    <t>Friday 6 Nov</t>
-  </si>
-  <si>
-    <t>Friday 13 Nov</t>
   </si>
 </sst>
 </file>
@@ -3776,1360 +3705,4 @@
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <legacyDrawing r:id="anysvml"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I55"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
-      <selection activeCell="L22" sqref="L22:L23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col customWidth="1" max="1" min="1" style="58" width="14.5703125"/>
-    <col customWidth="1" max="5" min="2" style="58" width="9.7109375"/>
-    <col customWidth="1" max="6" min="6" style="58" width="14.5703125"/>
-    <col customWidth="1" max="9" min="7" style="58" width="8.28515625"/>
-  </cols>
-  <sheetData>
-    <row customHeight="1" ht="17.25" r="1" s="58" spans="1:9">
-      <c r="A1" s="76" t="s">
-        <v>65</v>
-      </c>
-      <c r="B1" s="76" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="76" t="n"/>
-      <c r="D1" s="76" t="n"/>
-      <c r="F1" s="78" t="s">
-        <v>67</v>
-      </c>
-      <c r="G1" s="76" t="s">
-        <v>66</v>
-      </c>
-      <c r="H1" s="76" t="n"/>
-      <c r="I1" s="76" t="n"/>
-    </row>
-    <row customHeight="1" ht="17.25" r="2" s="58" spans="1:9">
-      <c r="A2" s="81" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="83" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="83" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="83" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" s="82" t="s">
-        <v>69</v>
-      </c>
-      <c r="G2" s="83" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="83" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" s="83" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="3" s="58" spans="1:9">
-      <c r="A3" s="83" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="83" t="n">
-        <v>29</v>
-      </c>
-      <c r="C3" s="83" t="n">
-        <v>53</v>
-      </c>
-      <c r="D3" s="83" t="n">
-        <v>79</v>
-      </c>
-      <c r="F3" s="79" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="83" t="n">
-        <v>29</v>
-      </c>
-      <c r="H3" s="83" t="n">
-        <v>53</v>
-      </c>
-      <c r="I3" s="83" t="n">
-        <v>79</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="4" s="58" spans="1:9">
-      <c r="A4" s="83" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="83" t="n">
-        <v>53</v>
-      </c>
-      <c r="C4" s="83" t="n">
-        <v>53</v>
-      </c>
-      <c r="D4" s="83" t="n">
-        <v>49</v>
-      </c>
-      <c r="F4" s="79" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="83" t="n">
-        <v>53</v>
-      </c>
-      <c r="H4" s="83" t="n">
-        <v>53</v>
-      </c>
-      <c r="I4" s="83" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="5" s="58" spans="1:9">
-      <c r="A5" s="83" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="83" t="n">
-        <v>45</v>
-      </c>
-      <c r="D5" s="83" t="n">
-        <v>49</v>
-      </c>
-      <c r="F5" s="79" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="83" t="n">
-        <v>45</v>
-      </c>
-      <c r="I5" s="83" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="6" s="58" spans="1:9">
-      <c r="A6" s="83" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="83" t="n">
-        <v>22</v>
-      </c>
-      <c r="C6" s="83" t="n">
-        <v>45</v>
-      </c>
-      <c r="D6" s="83" t="n">
-        <v>98</v>
-      </c>
-      <c r="F6" s="79" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="83" t="n">
-        <v>22</v>
-      </c>
-      <c r="H6" s="83" t="n">
-        <v>45</v>
-      </c>
-      <c r="I6" s="83" t="n">
-        <v>98</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="7" s="58" spans="1:9">
-      <c r="A7" s="83" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="83" t="n">
-        <v>60</v>
-      </c>
-      <c r="C7" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" s="84" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="79" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="83" t="n">
-        <v>60</v>
-      </c>
-      <c r="H7" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="83" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="8" s="58" spans="1:9">
-      <c r="A8" s="83" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="83" t="n">
-        <v>18</v>
-      </c>
-      <c r="C8" s="83" t="n">
-        <v>33</v>
-      </c>
-      <c r="D8" s="83" t="n">
-        <v>66</v>
-      </c>
-      <c r="F8" s="79" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="83" t="n">
-        <v>18</v>
-      </c>
-      <c r="H8" s="83" t="n">
-        <v>33</v>
-      </c>
-      <c r="I8" s="83" t="n">
-        <v>66</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="9" s="58" spans="1:9">
-      <c r="A9" s="83" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" s="83" t="n">
-        <v>33</v>
-      </c>
-      <c r="D9" s="83" t="n">
-        <v>19</v>
-      </c>
-      <c r="F9" s="79" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="83" t="n">
-        <v>33</v>
-      </c>
-      <c r="I9" s="83" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="10" s="58" spans="1:9">
-      <c r="A10" s="83" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="83" t="n">
-        <v>53</v>
-      </c>
-      <c r="C10" s="83" t="n">
-        <v>35</v>
-      </c>
-      <c r="D10" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="79" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="83" t="n">
-        <v>53</v>
-      </c>
-      <c r="H10" s="83" t="n">
-        <v>35</v>
-      </c>
-      <c r="I10" s="83" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="11" s="58" spans="1:9">
-      <c r="A11" s="83" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="83" t="n">
-        <v>53</v>
-      </c>
-      <c r="C11" s="83" t="n">
-        <v>35</v>
-      </c>
-      <c r="D11" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="79" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="83" t="n">
-        <v>53</v>
-      </c>
-      <c r="H11" s="83" t="n">
-        <v>35</v>
-      </c>
-      <c r="I11" s="83" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="12" s="58" spans="1:9">
-      <c r="F12" s="80" t="n"/>
-    </row>
-    <row customHeight="1" ht="17.25" r="13" s="58" spans="1:9">
-      <c r="A13" s="81" t="s">
-        <v>70</v>
-      </c>
-      <c r="B13" s="83" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="83" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="83" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="82" t="s">
-        <v>71</v>
-      </c>
-      <c r="G13" s="83" t="s">
-        <v>0</v>
-      </c>
-      <c r="H13" s="83" t="s">
-        <v>36</v>
-      </c>
-      <c r="I13" s="83" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="14" s="58" spans="1:9">
-      <c r="A14" s="83" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" s="83" t="n">
-        <v>143</v>
-      </c>
-      <c r="F14" s="79" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" s="83" t="n">
-        <v>143</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="15" s="58" spans="1:9">
-      <c r="A15" s="83" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="83" t="n">
-        <v>45</v>
-      </c>
-      <c r="C15" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" s="83" t="n">
-        <v>112</v>
-      </c>
-      <c r="F15" s="79" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="83" t="n">
-        <v>45</v>
-      </c>
-      <c r="H15" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" s="83" t="n">
-        <v>112</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="16" s="58" spans="1:9">
-      <c r="A16" s="83" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="83" t="n">
-        <v>18</v>
-      </c>
-      <c r="C16" s="83" t="n">
-        <v>56</v>
-      </c>
-      <c r="D16" s="83" t="n">
-        <v>107</v>
-      </c>
-      <c r="F16" s="79" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="83" t="n">
-        <v>18</v>
-      </c>
-      <c r="H16" s="83" t="n">
-        <v>56</v>
-      </c>
-      <c r="I16" s="83" t="n">
-        <v>107</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="17" s="58" spans="1:9">
-      <c r="A17" s="83" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="83" t="n">
-        <v>27</v>
-      </c>
-      <c r="C17" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" s="83" t="n">
-        <v>139</v>
-      </c>
-      <c r="F17" s="79" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="83" t="n">
-        <v>27</v>
-      </c>
-      <c r="H17" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="I17" s="83" t="n">
-        <v>139</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="18" s="58" spans="1:9">
-      <c r="A18" s="83" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" s="84" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="83" t="n">
-        <v>103</v>
-      </c>
-      <c r="F18" s="79" t="s">
-        <v>22</v>
-      </c>
-      <c r="G18" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" s="84" t="s">
-        <v>45</v>
-      </c>
-      <c r="I18" s="83" t="n">
-        <v>103</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="19" s="58" spans="1:9">
-      <c r="A19" s="83" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="83" t="n">
-        <v>42</v>
-      </c>
-      <c r="C19" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" s="79" t="s">
-        <v>27</v>
-      </c>
-      <c r="G19" s="83" t="n">
-        <v>42</v>
-      </c>
-      <c r="H19" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" s="83" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="20" s="58" spans="1:9">
-      <c r="A20" s="83" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="83" t="n">
-        <v>42</v>
-      </c>
-      <c r="C20" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" s="83" t="n">
-        <v>108</v>
-      </c>
-      <c r="F20" s="79" t="s">
-        <v>29</v>
-      </c>
-      <c r="G20" s="83" t="n">
-        <v>42</v>
-      </c>
-      <c r="H20" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" s="83" t="n">
-        <v>108</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="21" s="58" spans="1:9">
-      <c r="A21" s="83" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="83" t="n">
-        <v>27</v>
-      </c>
-      <c r="C21" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" s="79" t="s">
-        <v>32</v>
-      </c>
-      <c r="G21" s="83" t="n">
-        <v>27</v>
-      </c>
-      <c r="H21" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="I21" s="83" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="22" s="58" spans="1:9">
-      <c r="A22" s="83" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="83" t="n">
-        <v>27</v>
-      </c>
-      <c r="C22" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" s="79" t="s">
-        <v>33</v>
-      </c>
-      <c r="G22" s="83" t="n">
-        <v>27</v>
-      </c>
-      <c r="H22" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="I22" s="83" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="23" s="58" spans="1:9">
-      <c r="F23" s="80" t="n"/>
-    </row>
-    <row customHeight="1" ht="17.25" r="24" s="58" spans="1:9">
-      <c r="A24" s="81" t="s">
-        <v>72</v>
-      </c>
-      <c r="B24" s="83" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" s="83" t="s">
-        <v>36</v>
-      </c>
-      <c r="D24" s="83" t="s">
-        <v>47</v>
-      </c>
-      <c r="F24" s="82" t="s">
-        <v>73</v>
-      </c>
-      <c r="G24" s="83" t="s">
-        <v>0</v>
-      </c>
-      <c r="H24" s="83" t="s">
-        <v>36</v>
-      </c>
-      <c r="I24" s="83" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="25" s="58" spans="1:9">
-      <c r="A25" s="83" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" s="83" t="n">
-        <v>29</v>
-      </c>
-      <c r="C25" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" s="83" t="n">
-        <v>79</v>
-      </c>
-      <c r="F25" s="79" t="s">
-        <v>10</v>
-      </c>
-      <c r="G25" s="83" t="n">
-        <v>29</v>
-      </c>
-      <c r="H25" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="I25" s="83" t="n">
-        <v>79</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="26" s="58" spans="1:9">
-      <c r="A26" s="83" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="83" t="n">
-        <v>53</v>
-      </c>
-      <c r="C26" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" s="79" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="83" t="n">
-        <v>53</v>
-      </c>
-      <c r="H26" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="I26" s="83" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="27" s="58" spans="1:9">
-      <c r="A27" s="83" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27" s="83" t="n">
-        <v>22</v>
-      </c>
-      <c r="C27" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D27" s="83" t="n">
-        <v>98</v>
-      </c>
-      <c r="F27" s="79" t="s">
-        <v>16</v>
-      </c>
-      <c r="G27" s="83" t="n">
-        <v>22</v>
-      </c>
-      <c r="H27" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="I27" s="83" t="n">
-        <v>98</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="28" s="58" spans="1:9">
-      <c r="A28" s="83" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" s="83" t="n">
-        <v>60</v>
-      </c>
-      <c r="C28" s="83" t="n">
-        <v>73</v>
-      </c>
-      <c r="D28" s="83" t="n">
-        <v>74</v>
-      </c>
-      <c r="F28" s="79" t="s">
-        <v>20</v>
-      </c>
-      <c r="G28" s="83" t="n">
-        <v>60</v>
-      </c>
-      <c r="H28" s="83" t="n">
-        <v>73</v>
-      </c>
-      <c r="I28" s="83" t="n">
-        <v>74</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="29" s="58" spans="1:9">
-      <c r="A29" s="83" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" s="83" t="n">
-        <v>60</v>
-      </c>
-      <c r="C29" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D29" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="F29" s="79" t="s">
-        <v>22</v>
-      </c>
-      <c r="G29" s="83" t="n">
-        <v>60</v>
-      </c>
-      <c r="H29" s="83" t="n">
-        <v>73</v>
-      </c>
-      <c r="I29" s="83" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="30" s="58" spans="1:9">
-      <c r="A30" s="83" t="s">
-        <v>27</v>
-      </c>
-      <c r="B30" s="83" t="n">
-        <v>38</v>
-      </c>
-      <c r="C30" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D30" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="F30" s="79" t="s">
-        <v>27</v>
-      </c>
-      <c r="G30" s="83" t="n">
-        <v>38</v>
-      </c>
-      <c r="H30" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="I30" s="83" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="31" s="58" spans="1:9">
-      <c r="A31" s="83" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="83" t="n">
-        <v>79</v>
-      </c>
-      <c r="C31" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D31" s="83" t="n">
-        <v>84</v>
-      </c>
-      <c r="F31" s="79" t="s">
-        <v>29</v>
-      </c>
-      <c r="G31" s="83" t="n">
-        <v>79</v>
-      </c>
-      <c r="H31" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="I31" s="83" t="n">
-        <v>84</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="32" s="58" spans="1:9">
-      <c r="A32" s="83" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="83" t="n">
-        <v>22</v>
-      </c>
-      <c r="C32" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D32" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="F32" s="79" t="s">
-        <v>32</v>
-      </c>
-      <c r="G32" s="83" t="n">
-        <v>22</v>
-      </c>
-      <c r="H32" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="I32" s="83" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="33" s="58" spans="1:9">
-      <c r="A33" s="83" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" s="83" t="n">
-        <v>22</v>
-      </c>
-      <c r="C33" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D33" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="F33" s="79" t="s">
-        <v>33</v>
-      </c>
-      <c r="G33" s="83" t="n">
-        <v>22</v>
-      </c>
-      <c r="H33" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="I33" s="83" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="34" s="58" spans="1:9">
-      <c r="F34" s="80" t="n"/>
-    </row>
-    <row customHeight="1" ht="17.25" r="35" s="58" spans="1:9">
-      <c r="A35" s="81" t="s">
-        <v>74</v>
-      </c>
-      <c r="B35" s="83" t="s">
-        <v>0</v>
-      </c>
-      <c r="C35" s="83" t="s">
-        <v>36</v>
-      </c>
-      <c r="D35" s="83" t="s">
-        <v>47</v>
-      </c>
-      <c r="F35" s="82" t="s">
-        <v>75</v>
-      </c>
-      <c r="G35" s="83" t="s">
-        <v>0</v>
-      </c>
-      <c r="H35" s="83" t="s">
-        <v>36</v>
-      </c>
-      <c r="I35" s="83" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="36" s="58" spans="1:9">
-      <c r="A36" s="83" t="s">
-        <v>10</v>
-      </c>
-      <c r="B36" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="C36" s="83" t="n">
-        <v>42</v>
-      </c>
-      <c r="D36" s="83" t="n">
-        <v>143</v>
-      </c>
-      <c r="F36" s="79" t="s">
-        <v>10</v>
-      </c>
-      <c r="G36" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="H36" s="83" t="n">
-        <v>42</v>
-      </c>
-      <c r="I36" s="83" t="n">
-        <v>143</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="37" s="58" spans="1:9">
-      <c r="A37" s="83" t="s">
-        <v>13</v>
-      </c>
-      <c r="B37" s="83" t="n">
-        <v>45</v>
-      </c>
-      <c r="C37" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D37" s="83" t="n">
-        <v>56</v>
-      </c>
-      <c r="F37" s="79" t="s">
-        <v>13</v>
-      </c>
-      <c r="G37" s="83" t="n">
-        <v>45</v>
-      </c>
-      <c r="H37" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="I37" s="83" t="n">
-        <v>56</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="38" s="58" spans="1:9">
-      <c r="A38" s="83" t="s">
-        <v>16</v>
-      </c>
-      <c r="B38" s="83" t="n">
-        <v>27</v>
-      </c>
-      <c r="C38" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D38" s="83" t="n">
-        <v>139</v>
-      </c>
-      <c r="F38" s="79" t="s">
-        <v>16</v>
-      </c>
-      <c r="G38" s="83" t="n">
-        <v>27</v>
-      </c>
-      <c r="H38" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="I38" s="83" t="n">
-        <v>139</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="39" s="58" spans="1:9">
-      <c r="A39" s="83" t="s">
-        <v>20</v>
-      </c>
-      <c r="B39" s="83" t="n">
-        <v>18</v>
-      </c>
-      <c r="C39" s="83" t="n">
-        <v>56</v>
-      </c>
-      <c r="D39" s="83" t="n">
-        <v>107</v>
-      </c>
-      <c r="F39" s="79" t="s">
-        <v>20</v>
-      </c>
-      <c r="G39" s="83" t="n">
-        <v>18</v>
-      </c>
-      <c r="H39" s="83" t="n">
-        <v>56</v>
-      </c>
-      <c r="I39" s="83" t="n">
-        <v>107</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="40" s="58" spans="1:9">
-      <c r="A40" s="83" t="s">
-        <v>22</v>
-      </c>
-      <c r="B40" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="C40" s="84" t="s">
-        <v>45</v>
-      </c>
-      <c r="D40" s="83" t="n">
-        <v>113</v>
-      </c>
-      <c r="F40" s="79" t="s">
-        <v>22</v>
-      </c>
-      <c r="G40" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="H40" s="84" t="s">
-        <v>45</v>
-      </c>
-      <c r="I40" s="83" t="n">
-        <v>113</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="41" s="58" spans="1:9">
-      <c r="A41" s="83" t="s">
-        <v>27</v>
-      </c>
-      <c r="B41" s="83" t="n">
-        <v>42</v>
-      </c>
-      <c r="C41" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D41" s="83" t="n">
-        <v>83</v>
-      </c>
-      <c r="F41" s="79" t="s">
-        <v>27</v>
-      </c>
-      <c r="G41" s="83" t="n">
-        <v>42</v>
-      </c>
-      <c r="H41" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="I41" s="83" t="n">
-        <v>83</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="42" s="58" spans="1:9">
-      <c r="A42" s="83" t="s">
-        <v>29</v>
-      </c>
-      <c r="B42" s="83" t="n">
-        <v>60</v>
-      </c>
-      <c r="C42" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D42" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="F42" s="79" t="s">
-        <v>29</v>
-      </c>
-      <c r="G42" s="83" t="n">
-        <v>60</v>
-      </c>
-      <c r="H42" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="I42" s="83" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="43" s="58" spans="1:9">
-      <c r="A43" s="83" t="s">
-        <v>32</v>
-      </c>
-      <c r="B43" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="C43" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D43" s="83" t="n">
-        <v>108</v>
-      </c>
-      <c r="F43" s="79" t="s">
-        <v>32</v>
-      </c>
-      <c r="G43" s="83" t="n">
-        <v>60</v>
-      </c>
-      <c r="H43" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="I43" s="83" t="n">
-        <v>108</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="44" s="58" spans="1:9">
-      <c r="A44" s="83" t="s">
-        <v>33</v>
-      </c>
-      <c r="B44" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="C44" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D44" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="F44" s="79" t="s">
-        <v>33</v>
-      </c>
-      <c r="G44" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="H44" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="I44" s="83" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="45" s="58" spans="1:9">
-      <c r="F45" s="80" t="n"/>
-    </row>
-    <row customHeight="1" ht="17.25" r="46" s="58" spans="1:9">
-      <c r="A46" s="81" t="s">
-        <v>76</v>
-      </c>
-      <c r="B46" s="83" t="s">
-        <v>0</v>
-      </c>
-      <c r="C46" s="83" t="s">
-        <v>36</v>
-      </c>
-      <c r="D46" s="83" t="s">
-        <v>47</v>
-      </c>
-      <c r="F46" s="82" t="s">
-        <v>77</v>
-      </c>
-      <c r="G46" s="83" t="s">
-        <v>0</v>
-      </c>
-      <c r="H46" s="83" t="s">
-        <v>36</v>
-      </c>
-      <c r="I46" s="83" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="47" s="58" spans="1:9">
-      <c r="A47" s="83" t="s">
-        <v>10</v>
-      </c>
-      <c r="B47" s="83" t="n">
-        <v>38</v>
-      </c>
-      <c r="C47" s="83" t="n">
-        <v>45</v>
-      </c>
-      <c r="D47" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="F47" s="79" t="s">
-        <v>10</v>
-      </c>
-      <c r="G47" s="83" t="n">
-        <v>38</v>
-      </c>
-      <c r="H47" s="83" t="n">
-        <v>45</v>
-      </c>
-      <c r="I47" s="83" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="48" s="58" spans="1:9">
-      <c r="A48" s="83" t="s">
-        <v>13</v>
-      </c>
-      <c r="B48" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="C48" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D48" s="83" t="n">
-        <v>96</v>
-      </c>
-      <c r="F48" s="79" t="s">
-        <v>13</v>
-      </c>
-      <c r="G48" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="H48" s="83" t="n">
-        <v>45</v>
-      </c>
-      <c r="I48" s="83" t="n">
-        <v>96</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="49" s="58" spans="1:9">
-      <c r="A49" s="83" t="s">
-        <v>16</v>
-      </c>
-      <c r="B49" s="83" t="n">
-        <v>29</v>
-      </c>
-      <c r="C49" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D49" s="83" t="n">
-        <v>84</v>
-      </c>
-      <c r="F49" s="79" t="s">
-        <v>16</v>
-      </c>
-      <c r="G49" s="83" t="n">
-        <v>29</v>
-      </c>
-      <c r="H49" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="I49" s="83" t="n">
-        <v>84</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="50" s="58" spans="1:9">
-      <c r="A50" s="83" t="s">
-        <v>20</v>
-      </c>
-      <c r="B50" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="C50" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D50" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="F50" s="79" t="s">
-        <v>20</v>
-      </c>
-      <c r="G50" s="83" t="n">
-        <v>29</v>
-      </c>
-      <c r="H50" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="I50" s="83" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="51" s="58" spans="1:9">
-      <c r="A51" s="83" t="s">
-        <v>22</v>
-      </c>
-      <c r="B51" s="83" t="n">
-        <v>51</v>
-      </c>
-      <c r="C51" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D51" s="83" t="n">
-        <v>103</v>
-      </c>
-      <c r="F51" s="79" t="s">
-        <v>22</v>
-      </c>
-      <c r="G51" s="83" t="n">
-        <v>51</v>
-      </c>
-      <c r="H51" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="I51" s="83" t="n">
-        <v>103</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="52" s="58" spans="1:9">
-      <c r="A52" s="83" t="s">
-        <v>27</v>
-      </c>
-      <c r="B52" s="83" t="n">
-        <v>42</v>
-      </c>
-      <c r="C52" s="83" t="n">
-        <v>65</v>
-      </c>
-      <c r="D52" s="83" t="n">
-        <v>113</v>
-      </c>
-      <c r="F52" s="79" t="s">
-        <v>27</v>
-      </c>
-      <c r="G52" s="83" t="n">
-        <v>42</v>
-      </c>
-      <c r="H52" s="83" t="n">
-        <v>65</v>
-      </c>
-      <c r="I52" s="83" t="n">
-        <v>113</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="53" s="58" spans="1:9">
-      <c r="A53" s="83" t="s">
-        <v>29</v>
-      </c>
-      <c r="B53" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="C53" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D53" s="83" t="n">
-        <v>38</v>
-      </c>
-      <c r="F53" s="79" t="s">
-        <v>29</v>
-      </c>
-      <c r="G53" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="H53" s="83" t="n">
-        <v>65</v>
-      </c>
-      <c r="I53" s="83" t="n">
-        <v>38</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="54" s="58" spans="1:9">
-      <c r="A54" s="83" t="s">
-        <v>32</v>
-      </c>
-      <c r="B54" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="C54" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D54" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="F54" s="79" t="s">
-        <v>32</v>
-      </c>
-      <c r="G54" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="H54" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="I54" s="83" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17.25" r="55" s="58" spans="1:9">
-      <c r="A55" s="83" t="s">
-        <v>33</v>
-      </c>
-      <c r="B55" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="C55" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="D55" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="F55" s="79" t="s">
-        <v>33</v>
-      </c>
-      <c r="G55" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="H55" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="I55" s="83" t="n">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <legacyDrawing r:id="anysvml"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
update dataframes, start changing db to 1nf
</commit_message>
<xml_diff>
--- a/data_analytics/data/Fixed_B0.02 B0.03 B0.04 Timetable.xlsx
+++ b/data_analytics/data/Fixed_B0.02 B0.03 B0.04 Timetable.xlsx
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="70">
   <si>
     <t>B0.02</t>
   </si>
@@ -136,6 +136,21 @@
   </si>
   <si>
     <t>Friday 6th</t>
+  </si>
+  <si>
+    <t>Monday 9th</t>
+  </si>
+  <si>
+    <t>Tuesday 10th</t>
+  </si>
+  <si>
+    <t>Wednesday 11th</t>
+  </si>
+  <si>
+    <t>Thursday 12th</t>
+  </si>
+  <si>
+    <t>Friday 13th</t>
   </si>
   <si>
     <t>9:00 - 10:00</t>
@@ -1629,34 +1644,34 @@
       <c r="K2" s="104" t="n"/>
       <c r="M2" s="99" t="n"/>
       <c r="N2" s="16" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="O2" s="36" t="s">
         <v>5</v>
       </c>
       <c r="P2" s="102" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="Q2" s="103" t="n"/>
       <c r="R2" s="102" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="S2" s="103" t="n"/>
       <c r="T2" s="102" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="U2" s="104" t="n"/>
       <c r="V2" s="102" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="W2" s="104" t="n"/>
     </row>
     <row customHeight="1" ht="41.25" r="3" s="58" spans="1:23">
       <c r="A3" s="83" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C3" s="41" t="n">
         <v>29</v>
@@ -1664,7 +1679,7 @@
       <c r="D3" s="21" t="n"/>
       <c r="E3" s="8" t="n"/>
       <c r="F3" s="40" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G3" s="41" t="n">
         <v>29</v>
@@ -1672,16 +1687,16 @@
       <c r="H3" s="21" t="n"/>
       <c r="I3" s="26" t="n"/>
       <c r="J3" s="17" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="K3" s="42" t="n">
         <v>38</v>
       </c>
       <c r="M3" s="83" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N3" s="17" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="O3" s="41" t="n">
         <v>29</v>
@@ -1689,7 +1704,7 @@
       <c r="P3" s="21" t="n"/>
       <c r="Q3" s="8" t="n"/>
       <c r="R3" s="40" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="S3" s="41" t="n">
         <v>29</v>
@@ -1697,7 +1712,7 @@
       <c r="T3" s="21" t="n"/>
       <c r="U3" s="26" t="n"/>
       <c r="V3" s="17" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="W3" s="42" t="n">
         <v>38</v>
@@ -1705,28 +1720,28 @@
     </row>
     <row customHeight="1" ht="41.25" r="4" s="58" spans="1:23">
       <c r="A4" s="83" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C4" s="41" t="n">
         <v>53</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E4" s="41" t="n">
         <v>45</v>
       </c>
       <c r="F4" s="40" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G4" s="41" t="n">
         <v>53</v>
       </c>
       <c r="H4" s="40" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I4" s="13" t="n">
         <v>45</v>
@@ -1734,28 +1749,28 @@
       <c r="J4" s="18" t="n"/>
       <c r="K4" s="33" t="n"/>
       <c r="M4" s="83" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="N4" s="17" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="O4" s="41" t="n">
         <v>53</v>
       </c>
       <c r="P4" s="40" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="Q4" s="41" t="n">
         <v>45</v>
       </c>
       <c r="R4" s="40" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="S4" s="41" t="n">
         <v>53</v>
       </c>
       <c r="T4" s="40" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="U4" s="13" t="n">
         <v>45</v>
@@ -1765,59 +1780,59 @@
     </row>
     <row customHeight="1" ht="41.25" r="5" s="58" spans="1:23">
       <c r="A5" s="83" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B5" s="18" t="n"/>
       <c r="C5" s="8" t="n"/>
       <c r="D5" s="40" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E5" s="41" t="n">
         <v>18</v>
       </c>
       <c r="F5" s="40" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G5" s="41" t="n">
         <v>22</v>
       </c>
       <c r="H5" s="40" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I5" s="13" t="n">
         <v>27</v>
       </c>
       <c r="J5" s="105" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="K5" s="95" t="n">
         <v>29</v>
       </c>
       <c r="M5" s="83" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="N5" s="18" t="n"/>
       <c r="O5" s="8" t="n"/>
       <c r="P5" s="40" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="Q5" s="41" t="n">
         <v>18</v>
       </c>
       <c r="R5" s="40" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="S5" s="41" t="n">
         <v>22</v>
       </c>
       <c r="T5" s="40" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="U5" s="13" t="n">
         <v>27</v>
       </c>
       <c r="V5" s="105" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="W5" s="95" t="n">
         <v>29</v>
@@ -1825,67 +1840,67 @@
     </row>
     <row customHeight="1" ht="41.25" r="6" s="58" spans="1:23">
       <c r="A6" s="83" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C6" s="9" t="n">
         <v>22</v>
       </c>
       <c r="D6" s="43" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E6" s="9" t="n">
         <v>27</v>
       </c>
       <c r="F6" s="43" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G6" s="9" t="n">
         <v>60</v>
       </c>
       <c r="H6" s="43" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="I6" s="44" t="n">
         <v>18</v>
       </c>
       <c r="J6" s="106" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="K6" s="96" t="n">
         <v>29</v>
       </c>
       <c r="M6" s="83" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N6" s="19" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="O6" s="9" t="n">
         <v>22</v>
       </c>
       <c r="P6" s="43" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="Q6" s="9" t="n">
         <v>27</v>
       </c>
       <c r="R6" s="43" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="S6" s="9" t="n">
         <v>60</v>
       </c>
       <c r="T6" s="43" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="U6" s="44" t="n">
         <v>18</v>
       </c>
       <c r="V6" s="106" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="W6" s="96" t="n">
         <v>29</v>
@@ -1893,10 +1908,10 @@
     </row>
     <row customHeight="1" ht="41.25" r="7" s="58" spans="1:23">
       <c r="A7" s="83" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C7" s="41" t="n">
         <v>60</v>
@@ -1904,28 +1919,28 @@
       <c r="D7" s="21" t="n"/>
       <c r="E7" s="8" t="n"/>
       <c r="F7" s="40" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="G7" s="41" t="n">
         <v>60</v>
       </c>
       <c r="H7" s="29" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="I7" s="27" t="n">
         <v>0</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="K7" s="42" t="n">
         <v>51</v>
       </c>
       <c r="M7" s="83" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="N7" s="17" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="O7" s="41" t="n">
         <v>60</v>
@@ -1933,19 +1948,19 @@
       <c r="P7" s="21" t="n"/>
       <c r="Q7" s="8" t="n"/>
       <c r="R7" s="40" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="S7" s="41" t="n">
         <v>60</v>
       </c>
       <c r="T7" s="29" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="U7" s="27" t="n">
         <v>0</v>
       </c>
       <c r="V7" s="17" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="W7" s="42" t="n">
         <v>51</v>
@@ -1953,67 +1968,67 @@
     </row>
     <row customHeight="1" ht="41.25" r="8" s="58" spans="1:23">
       <c r="A8" s="83" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C8" s="10" t="n">
         <v>18</v>
       </c>
       <c r="D8" s="105" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E8" s="97" t="n">
         <v>42</v>
       </c>
       <c r="F8" s="40" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G8" s="41" t="n">
         <v>38</v>
       </c>
       <c r="H8" s="40" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="I8" s="28" t="n">
         <v>42</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="K8" s="13" t="n">
         <v>42</v>
       </c>
       <c r="M8" s="83" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="N8" s="17" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="O8" s="10" t="n">
         <v>18</v>
       </c>
       <c r="P8" s="105" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="Q8" s="97" t="n">
         <v>42</v>
       </c>
       <c r="R8" s="40" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="S8" s="41" t="n">
         <v>38</v>
       </c>
       <c r="T8" s="40" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="U8" s="28" t="n">
         <v>42</v>
       </c>
       <c r="V8" s="17" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="W8" s="13" t="n">
         <v>42</v>
@@ -2021,24 +2036,24 @@
     </row>
     <row customHeight="1" ht="41.25" r="9" s="58" spans="1:23">
       <c r="A9" s="83" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B9" s="20" t="n"/>
       <c r="C9" s="11" t="n"/>
       <c r="D9" s="106" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E9" s="94" t="n">
         <v>42</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G9" s="9" t="n">
         <v>79</v>
       </c>
       <c r="H9" s="121" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="I9" s="95" t="n">
         <v>60</v>
@@ -2046,24 +2061,24 @@
       <c r="J9" s="34" t="n"/>
       <c r="K9" s="31" t="n"/>
       <c r="M9" s="83" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="N9" s="20" t="n"/>
       <c r="O9" s="11" t="n"/>
       <c r="P9" s="106" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="Q9" s="94" t="n">
         <v>42</v>
       </c>
       <c r="R9" s="24" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="S9" s="9" t="n">
         <v>79</v>
       </c>
       <c r="T9" s="121" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="U9" s="95" t="n">
         <v>60</v>
@@ -2073,28 +2088,28 @@
     </row>
     <row customHeight="1" ht="41.25" r="10" s="58" spans="1:23">
       <c r="A10" s="83" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B10" s="105" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C10" s="93" t="n">
         <v>53</v>
       </c>
       <c r="D10" s="121" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E10" s="93" t="n">
         <v>27</v>
       </c>
       <c r="F10" s="121" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G10" s="93" t="n">
         <v>22</v>
       </c>
       <c r="H10" s="122" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="I10" s="96" t="n">
         <v>60</v>
@@ -2102,28 +2117,28 @@
       <c r="J10" s="34" t="n"/>
       <c r="K10" s="31" t="n"/>
       <c r="M10" s="83" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="N10" s="105" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="O10" s="93" t="n">
         <v>53</v>
       </c>
       <c r="P10" s="121" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="Q10" s="93" t="n">
         <v>27</v>
       </c>
       <c r="R10" s="121" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="S10" s="93" t="n">
         <v>22</v>
       </c>
       <c r="T10" s="122" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="U10" s="96" t="n">
         <v>60</v>
@@ -2133,22 +2148,22 @@
     </row>
     <row customHeight="1" ht="41.25" r="11" s="58" spans="1:23">
       <c r="A11" s="83" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B11" s="106" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C11" s="94" t="n">
         <v>53</v>
       </c>
       <c r="D11" s="122" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E11" s="94" t="n">
         <v>27</v>
       </c>
       <c r="F11" s="122" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G11" s="94" t="n">
         <v>22</v>
@@ -2158,22 +2173,22 @@
       <c r="J11" s="20" t="n"/>
       <c r="K11" s="32" t="n"/>
       <c r="M11" s="83" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="N11" s="106" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="O11" s="94" t="n">
         <v>53</v>
       </c>
       <c r="P11" s="122" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="Q11" s="94" t="n">
         <v>27</v>
       </c>
       <c r="R11" s="122" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="S11" s="94" t="n">
         <v>22</v>
@@ -2186,7 +2201,7 @@
     <row customHeight="1" ht="41.25" r="12" s="58" spans="1:23"/>
     <row customHeight="1" ht="41.25" r="13" s="58" spans="1:23">
       <c r="B13" s="59" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C13" s="1" t="n"/>
       <c r="D13" s="1" t="n"/>
@@ -2208,7 +2223,7 @@
     </row>
     <row customHeight="1" ht="41.25" r="14" s="58" spans="1:23">
       <c r="B14" s="60" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D14" s="86" t="n"/>
       <c r="E14" s="86" t="n"/>
@@ -2327,7 +2342,7 @@
   <sheetData>
     <row customHeight="1" ht="41.25" r="1" s="58" spans="1:23">
       <c r="A1" s="130" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B1" s="37" t="s">
         <v>1</v>
@@ -2344,7 +2359,7 @@
       <c r="J1" s="132" t="n"/>
       <c r="K1" s="133" t="n"/>
       <c r="M1" s="130" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="N1" s="37" t="s">
         <v>3</v>
@@ -2387,34 +2402,34 @@
       <c r="K2" s="136" t="n"/>
       <c r="M2" s="131" t="n"/>
       <c r="N2" s="38" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="O2" s="39" t="s">
         <v>5</v>
       </c>
       <c r="P2" s="134" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="Q2" s="135" t="n"/>
       <c r="R2" s="134" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="S2" s="135" t="n"/>
       <c r="T2" s="134" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="U2" s="136" t="n"/>
       <c r="V2" s="134" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="W2" s="136" t="n"/>
     </row>
     <row customHeight="1" ht="41.25" r="3" s="58" spans="1:23">
       <c r="A3" s="83" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B3" s="105" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C3" s="123" t="n">
         <v>53</v>
@@ -2422,28 +2437,28 @@
       <c r="D3" s="54" t="n"/>
       <c r="E3" s="57" t="n"/>
       <c r="F3" s="29" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G3" s="5" t="n">
         <v>0</v>
       </c>
       <c r="H3" s="40" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="I3" s="42" t="n">
         <v>42</v>
       </c>
       <c r="J3" s="105" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="K3" s="116" t="n">
         <v>45</v>
       </c>
       <c r="M3" s="83" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N3" s="105" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="O3" s="123" t="n">
         <v>53</v>
@@ -2451,19 +2466,19 @@
       <c r="P3" s="54" t="n"/>
       <c r="Q3" s="57" t="n"/>
       <c r="R3" s="29" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="S3" s="5" t="n">
         <v>0</v>
       </c>
       <c r="T3" s="40" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="U3" s="42" t="n">
         <v>42</v>
       </c>
       <c r="V3" s="105" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="W3" s="116" t="n">
         <v>45</v>
@@ -2471,10 +2486,10 @@
     </row>
     <row customHeight="1" ht="41.25" r="4" s="58" spans="1:23">
       <c r="A4" s="83" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B4" s="106" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C4" s="124" t="n">
         <v>53</v>
@@ -2482,7 +2497,7 @@
       <c r="D4" s="46" t="n"/>
       <c r="E4" s="6" t="n"/>
       <c r="F4" s="117" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G4" s="111" t="n">
         <v>0</v>
@@ -2490,16 +2505,16 @@
       <c r="H4" s="54" t="n"/>
       <c r="I4" s="55" t="n"/>
       <c r="J4" s="106" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="K4" s="115" t="n">
         <v>45</v>
       </c>
       <c r="M4" s="83" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="N4" s="106" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="O4" s="124" t="n">
         <v>53</v>
@@ -2507,7 +2522,7 @@
       <c r="P4" s="46" t="n"/>
       <c r="Q4" s="6" t="n"/>
       <c r="R4" s="117" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="S4" s="111" t="n">
         <v>0</v>
@@ -2515,7 +2530,7 @@
       <c r="T4" s="54" t="n"/>
       <c r="U4" s="55" t="n"/>
       <c r="V4" s="106" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="W4" s="115" t="n">
         <v>45</v>
@@ -2523,22 +2538,22 @@
     </row>
     <row customHeight="1" ht="41.25" r="5" s="58" spans="1:23">
       <c r="A5" s="83" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B5" s="105" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C5" s="123" t="n">
         <v>45</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E5" s="41" t="n">
         <v>56</v>
       </c>
       <c r="F5" s="118" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G5" s="112" t="n">
         <v>0</v>
@@ -2546,28 +2561,28 @@
       <c r="H5" s="46" t="n"/>
       <c r="I5" s="56" t="n"/>
       <c r="J5" s="125" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K5" s="127" t="n">
         <v>0</v>
       </c>
       <c r="M5" s="83" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="N5" s="105" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="O5" s="123" t="n">
         <v>45</v>
       </c>
       <c r="P5" s="40" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="Q5" s="41" t="n">
         <v>56</v>
       </c>
       <c r="R5" s="118" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="S5" s="112" t="n">
         <v>0</v>
@@ -2575,7 +2590,7 @@
       <c r="T5" s="46" t="n"/>
       <c r="U5" s="56" t="n"/>
       <c r="V5" s="125" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="W5" s="127" t="n">
         <v>0</v>
@@ -2583,10 +2598,10 @@
     </row>
     <row customHeight="1" ht="41.25" r="6" s="58" spans="1:23">
       <c r="A6" s="83" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B6" s="106" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C6" s="124" t="n">
         <v>45</v>
@@ -2594,28 +2609,28 @@
       <c r="D6" s="46" t="n"/>
       <c r="E6" s="6" t="n"/>
       <c r="F6" s="121" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="G6" s="123" t="n">
         <v>73</v>
       </c>
       <c r="H6" s="43" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="I6" s="44" t="n">
         <v>56</v>
       </c>
       <c r="J6" s="126" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K6" s="128" t="n">
         <v>0</v>
       </c>
       <c r="M6" s="83" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N6" s="106" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="O6" s="124" t="n">
         <v>45</v>
@@ -2623,19 +2638,19 @@
       <c r="P6" s="46" t="n"/>
       <c r="Q6" s="6" t="n"/>
       <c r="R6" s="121" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="S6" s="123" t="n">
         <v>73</v>
       </c>
       <c r="T6" s="43" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="U6" s="44" t="n">
         <v>56</v>
       </c>
       <c r="V6" s="126" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="W6" s="128" t="n">
         <v>0</v>
@@ -2643,62 +2658,62 @@
     </row>
     <row customHeight="1" ht="41.25" r="7" s="58" spans="1:23">
       <c r="A7" s="83" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B7" s="18" t="n"/>
       <c r="C7" s="8" t="n"/>
       <c r="D7" s="45" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E7" s="41" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F7" s="122" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="G7" s="124" t="n">
         <v>73</v>
       </c>
       <c r="H7" s="45" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="I7" s="61" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="J7" s="18" t="n"/>
       <c r="K7" s="26" t="n"/>
       <c r="M7" s="83" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="N7" s="18" t="n"/>
       <c r="O7" s="8" t="n"/>
       <c r="P7" s="45" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="Q7" s="41" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="R7" s="122" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="S7" s="124" t="n">
         <v>73</v>
       </c>
       <c r="T7" s="45" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="U7" s="61" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="V7" s="18" t="n"/>
       <c r="W7" s="26" t="n"/>
     </row>
     <row customHeight="1" ht="41.25" r="8" s="58" spans="1:23">
       <c r="A8" s="83" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B8" s="105" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C8" s="114" t="n">
         <v>33</v>
@@ -2706,28 +2721,28 @@
       <c r="D8" s="47" t="n"/>
       <c r="E8" s="48" t="n"/>
       <c r="F8" s="109" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G8" s="111" t="n">
         <v>0</v>
       </c>
       <c r="H8" s="29" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="I8" s="62" t="n">
         <v>0</v>
       </c>
       <c r="J8" s="105" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="K8" s="114" t="n">
         <v>65</v>
       </c>
       <c r="M8" s="83" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="N8" s="105" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="O8" s="114" t="n">
         <v>33</v>
@@ -2735,19 +2750,19 @@
       <c r="P8" s="47" t="n"/>
       <c r="Q8" s="48" t="n"/>
       <c r="R8" s="109" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="S8" s="111" t="n">
         <v>0</v>
       </c>
       <c r="T8" s="29" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="U8" s="62" t="n">
         <v>0</v>
       </c>
       <c r="V8" s="105" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="W8" s="114" t="n">
         <v>65</v>
@@ -2755,10 +2770,10 @@
     </row>
     <row customHeight="1" ht="41.25" r="9" s="58" spans="1:23">
       <c r="A9" s="83" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B9" s="106" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C9" s="108" t="n">
         <v>33</v>
@@ -2766,28 +2781,28 @@
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="50" t="n"/>
       <c r="F9" s="110" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G9" s="112" t="n">
         <v>0</v>
       </c>
       <c r="H9" s="29" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="I9" s="62" t="n">
         <v>0</v>
       </c>
       <c r="J9" s="113" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="K9" s="115" t="n">
         <v>65</v>
       </c>
       <c r="M9" s="83" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="N9" s="106" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="O9" s="108" t="n">
         <v>33</v>
@@ -2795,19 +2810,19 @@
       <c r="P9" s="49" t="n"/>
       <c r="Q9" s="50" t="n"/>
       <c r="R9" s="110" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="S9" s="112" t="n">
         <v>0</v>
       </c>
       <c r="T9" s="29" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="U9" s="62" t="n">
         <v>0</v>
       </c>
       <c r="V9" s="113" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="W9" s="115" t="n">
         <v>65</v>
@@ -2815,10 +2830,10 @@
     </row>
     <row customHeight="1" ht="41.25" r="10" s="58" spans="1:23">
       <c r="A10" s="83" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B10" s="105" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C10" s="123" t="n">
         <v>35</v>
@@ -2828,7 +2843,7 @@
       <c r="F10" s="51" t="n"/>
       <c r="G10" s="52" t="n"/>
       <c r="H10" s="109" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="I10" s="129" t="n">
         <v>0</v>
@@ -2836,10 +2851,10 @@
       <c r="J10" s="34" t="n"/>
       <c r="K10" s="31" t="n"/>
       <c r="M10" s="83" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="N10" s="105" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="O10" s="123" t="n">
         <v>35</v>
@@ -2849,7 +2864,7 @@
       <c r="R10" s="51" t="n"/>
       <c r="S10" s="52" t="n"/>
       <c r="T10" s="109" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="U10" s="129" t="n">
         <v>0</v>
@@ -2859,10 +2874,10 @@
     </row>
     <row customHeight="1" ht="41.25" r="11" s="58" spans="1:23">
       <c r="A11" s="83" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B11" s="106" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C11" s="124" t="n">
         <v>35</v>
@@ -2872,7 +2887,7 @@
       <c r="F11" s="53" t="n"/>
       <c r="G11" s="50" t="n"/>
       <c r="H11" s="110" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="I11" s="128" t="n">
         <v>0</v>
@@ -2880,10 +2895,10 @@
       <c r="J11" s="20" t="n"/>
       <c r="K11" s="32" t="n"/>
       <c r="M11" s="83" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="N11" s="106" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="O11" s="124" t="n">
         <v>35</v>
@@ -2893,7 +2908,7 @@
       <c r="R11" s="53" t="n"/>
       <c r="S11" s="50" t="n"/>
       <c r="T11" s="110" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="U11" s="128" t="n">
         <v>0</v>
@@ -2904,7 +2919,7 @@
     <row customHeight="1" ht="41.25" r="12" s="58" spans="1:23"/>
     <row customHeight="1" ht="41.25" r="13" s="58" spans="1:23">
       <c r="B13" s="59" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C13" s="1" t="n"/>
       <c r="D13" s="1" t="n"/>
@@ -2926,7 +2941,7 @@
     </row>
     <row customHeight="1" ht="41.25" r="14" s="58" spans="1:23">
       <c r="B14" s="60" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D14" s="86" t="n"/>
       <c r="E14" s="86" t="n"/>
@@ -3064,13 +3079,13 @@
   <sheetData>
     <row customHeight="1" ht="41.25" r="1" s="58" spans="1:23">
       <c r="A1" s="143" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B1" s="73" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="145" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D1" s="145" t="n"/>
       <c r="E1" s="145" t="n"/>
@@ -3081,13 +3096,13 @@
       <c r="J1" s="145" t="n"/>
       <c r="K1" s="146" t="n"/>
       <c r="M1" s="143" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="N1" s="73" t="s">
         <v>3</v>
       </c>
       <c r="O1" s="145" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="P1" s="145" t="n"/>
       <c r="Q1" s="145" t="n"/>
@@ -3124,52 +3139,52 @@
       <c r="K2" s="149" t="n"/>
       <c r="M2" s="144" t="n"/>
       <c r="N2" s="74" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="O2" s="75" t="s">
         <v>5</v>
       </c>
       <c r="P2" s="141" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="Q2" s="147" t="n"/>
       <c r="R2" s="141" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="S2" s="147" t="n"/>
       <c r="T2" s="141" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="U2" s="142" t="n"/>
       <c r="V2" s="141" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="W2" s="142" t="n"/>
     </row>
     <row customHeight="1" ht="41.25" r="3" s="58" spans="1:23">
       <c r="A3" s="83" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B3" s="65" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C3" s="63" t="n">
         <v>79</v>
       </c>
       <c r="D3" s="67" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E3" s="63" t="n">
         <v>143</v>
       </c>
       <c r="F3" s="67" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G3" s="63" t="n">
         <v>79</v>
       </c>
       <c r="H3" s="65" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="I3" s="63" t="n">
         <v>143</v>
@@ -3177,28 +3192,28 @@
       <c r="J3" s="66" t="n"/>
       <c r="K3" s="64" t="n"/>
       <c r="M3" s="83" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N3" s="65" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="O3" s="63" t="n">
         <v>79</v>
       </c>
       <c r="P3" s="67" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="Q3" s="63" t="n">
         <v>143</v>
       </c>
       <c r="R3" s="67" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="S3" s="63" t="n">
         <v>79</v>
       </c>
       <c r="T3" s="65" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="U3" s="63" t="n">
         <v>143</v>
@@ -3208,16 +3223,16 @@
     </row>
     <row customHeight="1" ht="41.25" r="4" s="58" spans="1:23">
       <c r="A4" s="83" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B4" s="137" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C4" s="139" t="n">
         <v>49</v>
       </c>
       <c r="D4" s="65" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="E4" s="63" t="n">
         <v>112</v>
@@ -3225,24 +3240,24 @@
       <c r="F4" s="66" t="n"/>
       <c r="G4" s="64" t="n"/>
       <c r="H4" s="65" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="I4" s="63" t="n">
         <v>56</v>
       </c>
       <c r="J4" s="65" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="K4" s="63" t="n">
         <v>96</v>
       </c>
       <c r="M4" s="83" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="N4" s="69" t="n"/>
       <c r="O4" s="70" t="n"/>
       <c r="P4" s="65" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="Q4" s="63" t="n">
         <v>112</v>
@@ -3250,13 +3265,13 @@
       <c r="R4" s="66" t="n"/>
       <c r="S4" s="64" t="n"/>
       <c r="T4" s="65" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="U4" s="63" t="n">
         <v>56</v>
       </c>
       <c r="V4" s="65" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="W4" s="63" t="n">
         <v>96</v>
@@ -3264,63 +3279,63 @@
     </row>
     <row customHeight="1" ht="41.25" r="5" s="58" spans="1:23">
       <c r="A5" s="83" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B5" s="138" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C5" s="140" t="n">
         <v>49</v>
       </c>
       <c r="D5" s="65" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E5" s="63" t="n">
         <v>107</v>
       </c>
       <c r="F5" s="65" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="G5" s="63" t="n">
         <v>98</v>
       </c>
       <c r="H5" s="65" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="I5" s="63" t="n">
         <v>139</v>
       </c>
       <c r="J5" s="65" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="K5" s="63" t="n">
         <v>84</v>
       </c>
       <c r="M5" s="83" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="N5" s="68" t="n"/>
       <c r="O5" s="71" t="n"/>
       <c r="P5" s="65" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="Q5" s="63" t="n">
         <v>107</v>
       </c>
       <c r="R5" s="65" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="S5" s="63" t="n">
         <v>98</v>
       </c>
       <c r="T5" s="65" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="U5" s="63" t="n">
         <v>139</v>
       </c>
       <c r="V5" s="65" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="W5" s="63" t="n">
         <v>84</v>
@@ -3328,28 +3343,28 @@
     </row>
     <row customHeight="1" ht="41.25" r="6" s="58" spans="1:23">
       <c r="A6" s="83" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B6" s="65" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C6" s="63" t="n">
         <v>98</v>
       </c>
       <c r="D6" s="65" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="E6" s="63" t="n">
         <v>139</v>
       </c>
       <c r="F6" s="65" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="G6" s="63" t="n">
         <v>74</v>
       </c>
       <c r="H6" s="65" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="I6" s="63" t="n">
         <v>107</v>
@@ -3357,28 +3372,28 @@
       <c r="J6" s="66" t="n"/>
       <c r="K6" s="64" t="n"/>
       <c r="M6" s="83" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N6" s="65" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="O6" s="63" t="n">
         <v>98</v>
       </c>
       <c r="P6" s="65" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="Q6" s="63" t="n">
         <v>139</v>
       </c>
       <c r="R6" s="65" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="S6" s="63" t="n">
         <v>74</v>
       </c>
       <c r="T6" s="65" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="U6" s="63" t="n">
         <v>107</v>
@@ -3388,16 +3403,16 @@
     </row>
     <row customHeight="1" ht="41.25" r="7" s="58" spans="1:23">
       <c r="A7" s="83" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B7" s="65" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C7" s="72" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D7" s="65" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E7" s="63" t="n">
         <v>103</v>
@@ -3405,24 +3420,24 @@
       <c r="F7" s="66" t="n"/>
       <c r="G7" s="64" t="n"/>
       <c r="H7" s="65" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="I7" s="63" t="n">
         <v>113</v>
       </c>
       <c r="J7" s="65" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="K7" s="63" t="n">
         <v>103</v>
       </c>
       <c r="M7" s="83" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="N7" s="66" t="n"/>
       <c r="O7" s="64" t="n"/>
       <c r="P7" s="65" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="Q7" s="63" t="n">
         <v>103</v>
@@ -3430,13 +3445,13 @@
       <c r="R7" s="66" t="n"/>
       <c r="S7" s="64" t="n"/>
       <c r="T7" s="65" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="U7" s="63" t="n">
         <v>113</v>
       </c>
       <c r="V7" s="65" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="W7" s="63" t="n">
         <v>103</v>
@@ -3444,16 +3459,16 @@
     </row>
     <row customHeight="1" ht="41.25" r="8" s="58" spans="1:23">
       <c r="A8" s="83" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B8" s="65" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C8" s="63" t="n">
         <v>66</v>
       </c>
       <c r="D8" s="65" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E8" s="63" t="n">
         <v>0</v>
@@ -3461,28 +3476,28 @@
       <c r="F8" s="66" t="n"/>
       <c r="G8" s="64" t="n"/>
       <c r="H8" s="65" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="I8" s="63" t="n">
         <v>83</v>
       </c>
       <c r="J8" s="65" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="K8" s="63" t="n">
         <v>113</v>
       </c>
       <c r="M8" s="83" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="N8" s="65" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="O8" s="63" t="n">
         <v>66</v>
       </c>
       <c r="P8" s="65" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="Q8" s="63" t="n">
         <v>0</v>
@@ -3490,13 +3505,13 @@
       <c r="R8" s="66" t="n"/>
       <c r="S8" s="64" t="n"/>
       <c r="T8" s="65" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="U8" s="63" t="n">
         <v>83</v>
       </c>
       <c r="V8" s="65" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="W8" s="63" t="n">
         <v>113</v>
@@ -3504,22 +3519,22 @@
     </row>
     <row customHeight="1" ht="41.25" r="9" s="58" spans="1:23">
       <c r="A9" s="83" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B9" s="65" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C9" s="63" t="n">
         <v>19</v>
       </c>
       <c r="D9" s="65" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E9" s="63" t="n">
         <v>108</v>
       </c>
       <c r="F9" s="65" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="G9" s="63" t="n">
         <v>84</v>
@@ -3527,28 +3542,28 @@
       <c r="H9" s="66" t="n"/>
       <c r="I9" s="64" t="n"/>
       <c r="J9" s="65" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="K9" s="63" t="n">
         <v>38</v>
       </c>
       <c r="M9" s="83" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="N9" s="65" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="O9" s="63" t="n">
         <v>19</v>
       </c>
       <c r="P9" s="65" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="Q9" s="63" t="n">
         <v>108</v>
       </c>
       <c r="R9" s="65" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="S9" s="63" t="n">
         <v>84</v>
@@ -3556,7 +3571,7 @@
       <c r="T9" s="66" t="n"/>
       <c r="U9" s="64" t="n"/>
       <c r="V9" s="65" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="W9" s="63" t="n">
         <v>38</v>
@@ -3564,7 +3579,7 @@
     </row>
     <row customHeight="1" ht="41.25" r="10" s="58" spans="1:23">
       <c r="A10" s="83" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B10" s="66" t="n"/>
       <c r="C10" s="64" t="n"/>
@@ -3573,7 +3588,7 @@
       <c r="F10" s="66" t="n"/>
       <c r="G10" s="64" t="n"/>
       <c r="H10" s="65" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="I10" s="63" t="n">
         <v>108</v>
@@ -3581,7 +3596,7 @@
       <c r="J10" s="66" t="n"/>
       <c r="K10" s="64" t="n"/>
       <c r="M10" s="83" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="N10" s="66" t="n"/>
       <c r="O10" s="64" t="n"/>
@@ -3590,7 +3605,7 @@
       <c r="R10" s="66" t="n"/>
       <c r="S10" s="64" t="n"/>
       <c r="T10" s="65" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="U10" s="63" t="n">
         <v>108</v>
@@ -3600,7 +3615,7 @@
     </row>
     <row customHeight="1" ht="41.25" r="11" s="58" spans="1:23">
       <c r="A11" s="83" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B11" s="66" t="n"/>
       <c r="C11" s="64" t="n"/>
@@ -3613,7 +3628,7 @@
       <c r="J11" s="66" t="n"/>
       <c r="K11" s="64" t="n"/>
       <c r="M11" s="83" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="N11" s="66" t="n"/>
       <c r="O11" s="64" t="n"/>
@@ -3629,7 +3644,7 @@
     <row customHeight="1" ht="41.25" r="12" s="58" spans="1:23"/>
     <row customHeight="1" ht="41.25" r="13" s="58" spans="1:23">
       <c r="B13" s="59" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C13" s="1" t="n"/>
       <c r="D13" s="1" t="n"/>
@@ -3651,7 +3666,7 @@
     </row>
     <row customHeight="1" ht="41.25" r="14" s="58" spans="1:23">
       <c r="B14" s="60" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D14" s="86" t="n"/>
       <c r="E14" s="86" t="n"/>

</xml_diff>

<commit_message>
Fixed bins in predict_occupancy function in data_analytics/predict.py
</commit_message>
<xml_diff>
--- a/data_analytics/data/Fixed_B0.02 B0.03 B0.04 Timetable.xlsx
+++ b/data_analytics/data/Fixed_B0.02 B0.03 B0.04 Timetable.xlsx
@@ -1545,7 +1545,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -2298,12 +2298,12 @@
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" paperSize="9"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -3035,12 +3035,12 @@
     <mergeCell ref="V8:V9"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -3718,6 +3718,6 @@
     <mergeCell ref="R14:S14"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
</xml_diff>